<commit_message>
UNGA BUNGA CODE COMMIT
added .gitignore file
modified xl reader
create test functions for servants pool creation
added servants xl sheet
</commit_message>
<xml_diff>
--- a/Servants.xlsx
+++ b/Servants.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eyho Cao\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eyho Cao\Documents\GitHub\FATE-DOM-SERVANT-ROLLER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DC0BE93-475D-4E2B-81F8-C42165D5C0CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B6E3B1-7E22-45E1-B438-F1F18E53FEB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{0FE483FA-8B5F-46F5-A3A6-9B8E7CBE2095}"/>
   </bookViews>
@@ -788,7 +788,7 @@
   <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1492,7 +1492,7 @@
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>